<commit_message>
Mostly art and silk updates
add garbotnik
edit silk
add touchpad label
update condiment step
</commit_message>
<xml_diff>
--- a/Swadge-HW/Manufacturing Information/Hot Dog Quotation.xlsx
+++ b/Swadge-HW/Manufacturing Information/Hot Dog Quotation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eanthony\Documents\GitHub\Super-2025-Swadge-HW\Swadge-HW\Manufacturing Information\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A72B2350-05C9-420F-B46C-8129D0169F5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7B9EACE-13D5-49A0-8AE8-2E58CB330D8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PCB Specification" sheetId="5" r:id="rId1"/>
@@ -44,15 +44,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="513" uniqueCount="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="279">
   <si>
     <t>Your PCB Specification</t>
   </si>
   <si>
     <t>PCB Quantity</t>
-  </si>
-  <si>
-    <t>1000pcs</t>
   </si>
   <si>
     <t>Layer</t>
@@ -345,15 +342,6 @@
     <t>Black</t>
   </si>
   <si>
-    <t>1500pcs</t>
-  </si>
-  <si>
-    <t>*</t>
-  </si>
-  <si>
-    <t>*quote both HASL Lead Free and ENIG Finish</t>
-  </si>
-  <si>
     <t>BT1, BT2, BT3</t>
   </si>
   <si>
@@ -468,9 +456,6 @@
     <t>2.2μF</t>
   </si>
   <si>
-    <t>470μF</t>
-  </si>
-  <si>
     <t>4.7nF</t>
   </si>
   <si>
@@ -567,9 +552,6 @@
     <t>C_0603_1608Metric</t>
   </si>
   <si>
-    <t>C_Radial_D4_L5.4_P3.321</t>
-  </si>
-  <si>
     <t>4020PAD</t>
   </si>
   <si>
@@ -955,6 +937,33 @@
   </si>
   <si>
     <t>BOTTOM</t>
+  </si>
+  <si>
+    <t>725pcs</t>
+  </si>
+  <si>
+    <t>1725pcs</t>
+  </si>
+  <si>
+    <t>ENIG</t>
+  </si>
+  <si>
+    <t>Changelog:</t>
+  </si>
+  <si>
+    <t>Change PCB qty to 725 red + 1725 black, total qty 1450</t>
+  </si>
+  <si>
+    <t>Change surface finish to ENIG</t>
+  </si>
+  <si>
+    <t>Change C26 component</t>
+  </si>
+  <si>
+    <t>470uF</t>
+  </si>
+  <si>
+    <t>C_Radial_D6.3_L5.8_P5.34</t>
   </si>
 </sst>
 </file>
@@ -1159,7 +1168,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1226,6 +1235,22 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -1630,10 +1655,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1661,145 +1686,145 @@
         <v>1</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>72</v>
+        <v>270</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>1</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>2</v>
+        <v>271</v>
       </c>
       <c r="E2" s="1"/>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="10" t="s">
-        <v>4</v>
-      </c>
       <c r="C3" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="10" t="s">
         <v>3</v>
-      </c>
-      <c r="D3" s="10" t="s">
-        <v>4</v>
       </c>
       <c r="E3" s="1"/>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="10" t="s">
-        <v>6</v>
-      </c>
       <c r="C4" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="10" t="s">
         <v>5</v>
-      </c>
-      <c r="D4" s="10" t="s">
-        <v>6</v>
       </c>
       <c r="E4" s="1"/>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="10" t="s">
-        <v>8</v>
-      </c>
       <c r="C5" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="10" t="s">
         <v>7</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>8</v>
       </c>
       <c r="E5" s="1"/>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="10" t="s">
-        <v>10</v>
-      </c>
       <c r="C6" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="10" t="s">
         <v>9</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>10</v>
       </c>
       <c r="E6" s="1"/>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B7" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="13" t="s">
         <v>70</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="13" t="s">
-        <v>71</v>
       </c>
       <c r="E7" s="1"/>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>73</v>
+        <v>272</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>73</v>
+        <v>272</v>
       </c>
       <c r="E8" s="1"/>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="10" t="s">
-        <v>14</v>
-      </c>
       <c r="C9" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="10" t="s">
         <v>13</v>
-      </c>
-      <c r="D9" s="10" t="s">
-        <v>14</v>
       </c>
       <c r="E9" s="1"/>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="10" t="s">
-        <v>16</v>
-      </c>
       <c r="C10" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="10" t="s">
         <v>15</v>
-      </c>
-      <c r="D10" s="10" t="s">
-        <v>16</v>
       </c>
       <c r="E10" s="1"/>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B11" s="11">
         <v>1</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D11" s="11">
         <v>1</v>
@@ -1815,7 +1840,7 @@
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B13" s="20"/>
       <c r="C13" s="20"/>
@@ -1824,7 +1849,7 @@
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="21" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B14" s="20"/>
       <c r="C14" s="20"/>
@@ -1838,9 +1863,24 @@
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
     </row>
-    <row r="17" spans="2:2">
-      <c r="B17" t="s">
-        <v>74</v>
+    <row r="18" spans="2:2">
+      <c r="B18" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2">
+      <c r="B19" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2">
+      <c r="B20" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2">
+      <c r="B21" t="s">
+        <v>276</v>
       </c>
     </row>
   </sheetData>
@@ -1862,8 +1902,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L44"/>
   <sheetViews>
-    <sheetView topLeftCell="C15" workbookViewId="0">
-      <selection activeCell="L25" sqref="L25"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1880,7 +1920,7 @@
   <sheetData>
     <row r="1" spans="1:12" s="4" customFormat="1" ht="26.25">
       <c r="A1" s="22" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B1" s="22"/>
       <c r="C1" s="22"/>
@@ -1896,40 +1936,40 @@
     </row>
     <row r="2" spans="1:12" s="4" customFormat="1" ht="14.25">
       <c r="A2" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="C2" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="D2" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="E2" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="F2" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="G2" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="H2" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="I2" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="J2" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="K2" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="L2" s="5" t="s">
         <v>31</v>
-      </c>
-      <c r="L2" s="5" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:12" s="4" customFormat="1">
@@ -1937,19 +1977,19 @@
         <v>1</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C3" s="15">
         <v>3</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="E3" s="16">
         <v>2460</v>
       </c>
       <c r="F3" s="15" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="I3" s="15">
         <f>C3</f>
@@ -1958,7 +1998,7 @@
       <c r="J3" s="5"/>
       <c r="K3" s="15"/>
       <c r="L3" s="15" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
     </row>
     <row r="4" spans="1:12" s="4" customFormat="1">
@@ -1966,16 +2006,16 @@
         <v>2</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C4" s="15">
         <v>10</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="E4" s="16" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="F4" s="15"/>
       <c r="H4" s="15">
@@ -1985,7 +2025,7 @@
       <c r="I4" s="5"/>
       <c r="J4" s="5"/>
       <c r="K4" s="15" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="L4" s="15"/>
     </row>
@@ -1994,16 +2034,16 @@
         <v>3</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C5" s="15">
         <v>6</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="E5" s="16" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="F5" s="15"/>
       <c r="H5" s="15">
@@ -2013,7 +2053,7 @@
       <c r="I5" s="5"/>
       <c r="J5" s="5"/>
       <c r="K5" s="15" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="L5" s="15"/>
     </row>
@@ -2022,16 +2062,16 @@
         <v>4</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C6" s="15">
         <v>5</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E6" s="16" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="F6" s="15"/>
       <c r="H6" s="15">
@@ -2041,7 +2081,7 @@
       <c r="I6" s="5"/>
       <c r="J6" s="5"/>
       <c r="K6" s="15" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="L6" s="15"/>
     </row>
@@ -2050,16 +2090,16 @@
         <v>5</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C7" s="15">
         <v>1</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="E7" s="16" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="F7" s="15"/>
       <c r="H7" s="15">
@@ -2069,7 +2109,7 @@
       <c r="I7" s="5"/>
       <c r="J7" s="5"/>
       <c r="K7" s="15" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="L7" s="15"/>
     </row>
@@ -2078,16 +2118,16 @@
         <v>6</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C8" s="15">
         <v>1</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="E8" s="16" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="F8" s="15"/>
       <c r="H8" s="15">
@@ -2097,53 +2137,53 @@
       <c r="I8" s="5"/>
       <c r="J8" s="5"/>
       <c r="K8" s="15" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
       <c r="L8" s="15"/>
     </row>
-    <row r="9" spans="1:12" s="4" customFormat="1">
-      <c r="A9" s="5">
+    <row r="9" spans="1:12" s="26" customFormat="1">
+      <c r="A9" s="23">
         <v>7</v>
       </c>
-      <c r="B9" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="C9" s="15">
+      <c r="B9" s="24" t="s">
+        <v>76</v>
+      </c>
+      <c r="C9" s="24">
         <v>1</v>
       </c>
-      <c r="D9" s="15" t="s">
-        <v>113</v>
-      </c>
-      <c r="E9" s="16" t="s">
-        <v>146</v>
-      </c>
-      <c r="F9" s="15"/>
-      <c r="H9" s="15">
+      <c r="D9" s="24" t="s">
+        <v>277</v>
+      </c>
+      <c r="E9" s="25" t="s">
+        <v>278</v>
+      </c>
+      <c r="F9" s="24"/>
+      <c r="H9" s="24">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="I9" s="5"/>
-      <c r="J9" s="5"/>
-      <c r="K9" s="15" t="s">
-        <v>274</v>
-      </c>
-      <c r="L9" s="15"/>
+      <c r="I9" s="23"/>
+      <c r="J9" s="23"/>
+      <c r="K9" s="24" t="s">
+        <v>268</v>
+      </c>
+      <c r="L9" s="24"/>
     </row>
     <row r="10" spans="1:12" s="4" customFormat="1">
       <c r="A10" s="5">
         <v>8</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C10" s="15">
         <v>1</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="E10" s="16" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="F10" s="15"/>
       <c r="H10" s="15">
@@ -2153,7 +2193,7 @@
       <c r="I10" s="5"/>
       <c r="J10" s="5"/>
       <c r="K10" s="15" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="L10" s="15"/>
     </row>
@@ -2162,16 +2202,16 @@
         <v>9</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C11" s="15">
         <v>9</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="E11" s="16" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="F11" s="15"/>
       <c r="H11" s="15">
@@ -2181,7 +2221,7 @@
       <c r="I11" s="5"/>
       <c r="J11" s="5"/>
       <c r="K11" s="15" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="L11" s="15"/>
     </row>
@@ -2190,19 +2230,19 @@
         <v>10</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C12" s="15">
         <v>2</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="E12" s="16" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="F12" s="15" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="H12" s="15">
         <f t="shared" si="0"/>
@@ -2211,7 +2251,7 @@
       <c r="I12" s="5"/>
       <c r="J12" s="5"/>
       <c r="K12" s="15" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="L12" s="15"/>
     </row>
@@ -2220,19 +2260,19 @@
         <v>11</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C13" s="15">
         <v>1</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="E13" s="16" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="F13" s="15" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="H13" s="15">
         <f t="shared" si="0"/>
@@ -2241,7 +2281,7 @@
       <c r="I13" s="5"/>
       <c r="J13" s="5"/>
       <c r="K13" s="15" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="L13" s="15"/>
     </row>
@@ -2250,19 +2290,19 @@
         <v>12</v>
       </c>
       <c r="B14" s="15" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C14" s="15">
         <v>1</v>
       </c>
       <c r="D14" s="15" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="E14" s="16" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="F14" s="15" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="I14" s="15">
         <f>C14</f>
@@ -2270,7 +2310,7 @@
       </c>
       <c r="J14" s="5"/>
       <c r="K14" s="15" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="L14" s="15"/>
     </row>
@@ -2279,16 +2319,16 @@
         <v>13</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C15" s="15">
         <v>1</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="E15" s="16" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="F15" s="15"/>
       <c r="I15" s="15">
@@ -2297,7 +2337,7 @@
       </c>
       <c r="J15" s="5"/>
       <c r="K15" s="15" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="L15" s="15"/>
     </row>
@@ -2306,16 +2346,16 @@
         <v>14</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C16" s="15">
         <v>1</v>
       </c>
       <c r="D16" s="15" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="E16" s="16" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="F16" s="15"/>
       <c r="H16" s="15">
@@ -2325,7 +2365,7 @@
       <c r="I16" s="5"/>
       <c r="J16" s="5"/>
       <c r="K16" s="15" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="L16" s="15"/>
     </row>
@@ -2334,16 +2374,16 @@
         <v>15</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C17" s="15">
         <v>1</v>
       </c>
       <c r="D17" s="15" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="E17" s="16" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="F17" s="15"/>
       <c r="H17" s="15">
@@ -2353,7 +2393,7 @@
       <c r="I17" s="5"/>
       <c r="J17" s="5"/>
       <c r="K17" s="15" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="L17" s="15"/>
     </row>
@@ -2362,16 +2402,16 @@
         <v>16</v>
       </c>
       <c r="B18" s="15" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C18" s="15">
         <v>1</v>
       </c>
       <c r="D18" s="15" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="E18" s="16" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="F18" s="15"/>
       <c r="H18" s="15">
@@ -2381,7 +2421,7 @@
       <c r="I18" s="5"/>
       <c r="J18" s="5"/>
       <c r="K18" s="15" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="L18" s="15"/>
     </row>
@@ -2390,16 +2430,16 @@
         <v>17</v>
       </c>
       <c r="B19" s="15" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C19" s="15">
         <v>1</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="E19" s="16" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="F19" s="15"/>
       <c r="I19" s="15">
@@ -2408,10 +2448,10 @@
       </c>
       <c r="J19" s="5"/>
       <c r="K19" s="15" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="L19" s="15" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
     </row>
     <row r="20" spans="1:12" s="4" customFormat="1">
@@ -2419,16 +2459,16 @@
         <v>18</v>
       </c>
       <c r="B20" s="15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C20" s="15">
         <v>1</v>
       </c>
       <c r="D20" s="15" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="E20" s="16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F20" s="15"/>
       <c r="H20" s="15">
@@ -2438,7 +2478,7 @@
       <c r="I20" s="5"/>
       <c r="J20" s="5"/>
       <c r="K20" s="15" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="L20" s="15"/>
     </row>
@@ -2447,16 +2487,16 @@
         <v>19</v>
       </c>
       <c r="B21" s="15" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C21" s="15">
         <v>5</v>
       </c>
       <c r="D21" s="15" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="E21" s="16" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="F21" s="15"/>
       <c r="H21" s="15">
@@ -2466,7 +2506,7 @@
       <c r="I21" s="5"/>
       <c r="J21" s="5"/>
       <c r="K21" s="15" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="L21" s="15"/>
     </row>
@@ -2475,16 +2515,16 @@
         <v>20</v>
       </c>
       <c r="B22" s="15" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C22" s="15">
         <v>6</v>
       </c>
       <c r="D22" s="15" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="E22" s="16" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="F22" s="15"/>
       <c r="H22" s="15">
@@ -2494,7 +2534,7 @@
       <c r="I22" s="5"/>
       <c r="J22" s="5"/>
       <c r="K22" s="15" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="L22" s="15"/>
     </row>
@@ -2503,16 +2543,16 @@
         <v>21</v>
       </c>
       <c r="B23" s="15" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C23" s="15">
         <v>5</v>
       </c>
       <c r="D23" s="15" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="E23" s="16" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="F23" s="15"/>
       <c r="H23" s="15">
@@ -2522,7 +2562,7 @@
       <c r="I23" s="5"/>
       <c r="J23" s="5"/>
       <c r="K23" s="15" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="L23" s="15"/>
     </row>
@@ -2531,16 +2571,16 @@
         <v>22</v>
       </c>
       <c r="B24" s="15" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C24" s="15">
         <v>4</v>
       </c>
       <c r="D24" s="15" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="E24" s="16" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="F24" s="15"/>
       <c r="H24" s="15">
@@ -2550,7 +2590,7 @@
       <c r="I24" s="5"/>
       <c r="J24" s="5"/>
       <c r="K24" s="15" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="L24" s="15"/>
     </row>
@@ -2559,16 +2599,16 @@
         <v>23</v>
       </c>
       <c r="B25" s="15" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C25" s="15">
         <v>2</v>
       </c>
       <c r="D25" s="15" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="E25" s="16" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="F25" s="15"/>
       <c r="H25" s="15">
@@ -2578,7 +2618,7 @@
       <c r="I25" s="5"/>
       <c r="J25" s="5"/>
       <c r="K25" s="15" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="L25" s="15"/>
     </row>
@@ -2587,16 +2627,16 @@
         <v>24</v>
       </c>
       <c r="B26" s="15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C26" s="15">
         <v>1</v>
       </c>
       <c r="D26" s="15" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="E26" s="16" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="F26" s="15"/>
       <c r="H26" s="15">
@@ -2606,7 +2646,7 @@
       <c r="I26" s="5"/>
       <c r="J26" s="5"/>
       <c r="K26" s="15" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="L26" s="15"/>
     </row>
@@ -2615,16 +2655,16 @@
         <v>25</v>
       </c>
       <c r="B27" s="15" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C27" s="15">
         <v>2</v>
       </c>
       <c r="D27" s="15" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="E27" s="16" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="F27" s="15"/>
       <c r="H27" s="15">
@@ -2634,7 +2674,7 @@
       <c r="I27" s="5"/>
       <c r="J27" s="5"/>
       <c r="K27" s="15" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="L27" s="15"/>
     </row>
@@ -2643,16 +2683,16 @@
         <v>26</v>
       </c>
       <c r="B28" s="15" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C28" s="15">
         <v>1</v>
       </c>
       <c r="D28" s="15" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="E28" s="16" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="F28" s="15"/>
       <c r="H28" s="15">
@@ -2662,7 +2702,7 @@
       <c r="I28" s="5"/>
       <c r="J28" s="5"/>
       <c r="K28" s="15" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="L28" s="15"/>
     </row>
@@ -2671,19 +2711,19 @@
         <v>27</v>
       </c>
       <c r="B29" s="15" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C29" s="15">
         <v>6</v>
       </c>
       <c r="D29" s="15" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="E29" s="16" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="F29" s="15" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="H29" s="15">
         <f t="shared" si="1"/>
@@ -2692,10 +2732,10 @@
       <c r="I29" s="5"/>
       <c r="J29" s="5"/>
       <c r="K29" s="15" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="L29" s="15" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
     </row>
     <row r="30" spans="1:12">
@@ -2703,19 +2743,19 @@
         <v>28</v>
       </c>
       <c r="B30" s="15" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C30" s="15">
         <v>2</v>
       </c>
       <c r="D30" s="15" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="E30" s="16" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="F30" s="15" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="H30" s="15">
         <f t="shared" si="1"/>
@@ -2724,10 +2764,10 @@
       <c r="I30" s="5"/>
       <c r="J30" s="5"/>
       <c r="K30" s="15" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="L30" s="15" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
     </row>
     <row r="31" spans="1:12">
@@ -2735,19 +2775,19 @@
         <v>29</v>
       </c>
       <c r="B31" s="15" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C31" s="15">
         <v>1</v>
       </c>
       <c r="D31" s="15" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="E31" s="16" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="F31" s="15" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="I31" s="15">
         <f>C31</f>
@@ -2755,10 +2795,10 @@
       </c>
       <c r="J31" s="5"/>
       <c r="K31" s="15" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="L31" s="15" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
     </row>
     <row r="32" spans="1:12">
@@ -2766,16 +2806,16 @@
         <v>30</v>
       </c>
       <c r="B32" s="15" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="C32" s="15">
         <v>1</v>
       </c>
       <c r="D32" s="15" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="E32" s="16" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="F32" s="15"/>
       <c r="H32" s="15">
@@ -2785,10 +2825,10 @@
       <c r="I32" s="5"/>
       <c r="J32" s="5"/>
       <c r="K32" s="15" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="L32" s="15" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
     </row>
     <row r="33" spans="1:12">
@@ -2796,16 +2836,16 @@
         <v>31</v>
       </c>
       <c r="B33" s="15" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C33" s="15">
         <v>1</v>
       </c>
       <c r="D33" s="15" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="E33" s="16" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="F33" s="15"/>
       <c r="H33" s="15">
@@ -2815,7 +2855,7 @@
       <c r="I33" s="5"/>
       <c r="J33" s="5"/>
       <c r="K33" s="15" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="L33" s="15"/>
     </row>
@@ -2824,19 +2864,19 @@
         <v>32</v>
       </c>
       <c r="B34" s="15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C34" s="15">
         <v>1</v>
       </c>
       <c r="D34" s="15" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="E34" s="16" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="F34" s="15" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="I34" s="15">
         <f>C34</f>
@@ -2845,7 +2885,7 @@
       <c r="J34" s="5"/>
       <c r="K34" s="15"/>
       <c r="L34" s="15" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
     </row>
     <row r="35" spans="1:12">
@@ -2853,16 +2893,16 @@
         <v>33</v>
       </c>
       <c r="B35" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C35" s="15">
         <v>1</v>
       </c>
       <c r="D35" s="15" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="E35" s="16" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="F35" s="15"/>
       <c r="H35" s="15">
@@ -2872,10 +2912,10 @@
       <c r="I35" s="5"/>
       <c r="J35" s="5"/>
       <c r="K35" s="15" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="L35" s="15" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
     </row>
     <row r="36" spans="1:12">
@@ -2883,19 +2923,19 @@
         <v>34</v>
       </c>
       <c r="B36" s="15" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C36" s="15">
         <v>1</v>
       </c>
       <c r="D36" s="15" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="E36" s="16" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="F36" s="15" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="H36" s="15">
         <f t="shared" si="1"/>
@@ -2904,7 +2944,7 @@
       <c r="I36" s="5"/>
       <c r="J36" s="5"/>
       <c r="K36" s="15" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="L36" s="15"/>
     </row>
@@ -2913,16 +2953,16 @@
         <v>35</v>
       </c>
       <c r="B37" s="15" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C37" s="15">
         <v>1</v>
       </c>
       <c r="D37" s="15" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="E37" s="16" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="F37" s="15"/>
       <c r="H37" s="15">
@@ -2932,7 +2972,7 @@
       <c r="I37" s="5"/>
       <c r="J37" s="5"/>
       <c r="K37" s="15" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="L37" s="15"/>
     </row>
@@ -2941,16 +2981,16 @@
         <v>36</v>
       </c>
       <c r="B38" s="15" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="C38" s="15">
         <v>1</v>
       </c>
       <c r="D38" s="15" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="E38" s="16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F38" s="15"/>
       <c r="H38" s="15">
@@ -2960,7 +3000,7 @@
       <c r="I38" s="5"/>
       <c r="J38" s="5"/>
       <c r="K38" s="15" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="L38" s="15"/>
     </row>
@@ -2969,16 +3009,16 @@
         <v>37</v>
       </c>
       <c r="B39" s="15" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C39" s="15">
         <v>1</v>
       </c>
       <c r="D39" s="15" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="E39" s="16" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="F39" s="15"/>
       <c r="H39" s="15">
@@ -2988,7 +3028,7 @@
       <c r="I39" s="5"/>
       <c r="J39" s="5"/>
       <c r="K39" s="15" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="L39" s="15"/>
     </row>
@@ -2997,19 +3037,19 @@
         <v>38</v>
       </c>
       <c r="B40" s="15" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C40" s="15">
         <v>1</v>
       </c>
       <c r="D40" s="15" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="E40" s="16" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="F40" s="15" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="I40" s="15">
         <f>C40</f>
@@ -3017,7 +3057,7 @@
       </c>
       <c r="J40" s="5"/>
       <c r="K40" s="15" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="L40" s="15"/>
     </row>
@@ -3029,7 +3069,7 @@
       <c r="E41" s="6"/>
       <c r="F41" s="6"/>
       <c r="G41" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H41" s="7">
         <f>SUM(H3:H40)</f>
@@ -3060,7 +3100,7 @@
     <row r="43" spans="1:12" ht="15.75">
       <c r="A43" s="6"/>
       <c r="B43" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
@@ -3076,7 +3116,7 @@
     <row r="44" spans="1:12" ht="15.75">
       <c r="A44" s="6"/>
       <c r="B44" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
@@ -3103,7 +3143,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B2:B35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="T31" sqref="T31"/>
     </sheetView>
   </sheetViews>
@@ -3111,12 +3151,12 @@
   <sheetData>
     <row r="2" spans="2:2">
       <c r="B2" s="18" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
     </row>
     <row r="35" spans="2:2">
       <c r="B35" s="18" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
     </row>
   </sheetData>
@@ -3131,8 +3171,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F178"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -3148,27 +3188,27 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="2" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="B2" s="2">
         <v>2460</v>
@@ -3180,7 +3220,7 @@
         <v>-110.399922</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="F2" s="2">
         <v>100</v>
@@ -3188,7 +3228,7 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="2" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="B3" s="2">
         <v>2460</v>
@@ -3200,7 +3240,7 @@
         <v>-102.55</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="F3" s="2">
         <v>180</v>
@@ -3208,7 +3248,7 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="2" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="B4" s="2">
         <v>2460</v>
@@ -3220,7 +3260,7 @@
         <v>-107.749922</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="F4" s="2">
         <v>-100</v>
@@ -3228,10 +3268,10 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="2" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="C5" s="3">
         <v>157.64126099999999</v>
@@ -3240,7 +3280,7 @@
         <v>-69.009878</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="F5" s="2">
         <v>172</v>
@@ -3248,10 +3288,10 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="C6" s="3">
         <v>138.36150000000001</v>
@@ -3260,7 +3300,7 @@
         <v>-119.986</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="F6" s="2">
         <v>180</v>
@@ -3268,10 +3308,10 @@
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="C7" s="3">
         <v>150.69999999999999</v>
@@ -3280,7 +3320,7 @@
         <v>-82</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="F7" s="2">
         <v>-90</v>
@@ -3288,10 +3328,10 @@
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="C8" s="3">
         <v>136.94999999999999</v>
@@ -3300,7 +3340,7 @@
         <v>-123.1</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="F8" s="2">
         <v>180</v>
@@ -3308,10 +3348,10 @@
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="2" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="C9" s="3">
         <v>139.30000000000001</v>
@@ -3320,7 +3360,7 @@
         <v>-125.35</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="F9" s="2">
         <v>-90</v>
@@ -3328,10 +3368,10 @@
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="2" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="C10" s="3">
         <v>139.30000000000001</v>
@@ -3340,7 +3380,7 @@
         <v>-88.096500000000006</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="F10" s="2">
         <v>180</v>
@@ -3348,10 +3388,10 @@
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="2" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="C11" s="3">
         <v>129.35</v>
@@ -3360,7 +3400,7 @@
         <v>-88.837500000000006</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="F11" s="2">
         <v>90</v>
@@ -3368,10 +3408,10 @@
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="2" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="C12" s="3">
         <v>150.09549999999999</v>
@@ -3380,7 +3420,7 @@
         <v>-71.078000000000003</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="F12" s="2">
         <v>180</v>
@@ -3388,10 +3428,10 @@
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="2" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="C13" s="3">
         <v>120.3</v>
@@ -3400,7 +3440,7 @@
         <v>-117.3245</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="F13" s="2">
         <v>15</v>
@@ -3408,10 +3448,10 @@
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="2" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="C14" s="3">
         <v>142.5</v>
@@ -3420,7 +3460,7 @@
         <v>-91.05</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="F14" s="2">
         <v>0</v>
@@ -3428,10 +3468,10 @@
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="2" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="C15" s="3">
         <v>147.44999999999999</v>
@@ -3440,7 +3480,7 @@
         <v>-68.537499999999994</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="F15" s="2">
         <v>-90</v>
@@ -3448,10 +3488,10 @@
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="C16" s="3">
         <v>176.68152900000001</v>
@@ -3460,7 +3500,7 @@
         <v>-73.305937</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="F16" s="2">
         <v>-8</v>
@@ -3468,10 +3508,10 @@
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="C17" s="3">
         <v>172.1</v>
@@ -3480,7 +3520,7 @@
         <v>-91.8</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="F17" s="2">
         <v>180</v>
@@ -3488,10 +3528,10 @@
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="C18" s="3">
         <v>150.1</v>
@@ -3500,7 +3540,7 @@
         <v>-124.44</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="F18" s="2">
         <v>0</v>
@@ -3508,10 +3548,10 @@
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="2" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="C19" s="3">
         <v>142.1875</v>
@@ -3520,7 +3560,7 @@
         <v>-77.650000000000006</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="F19" s="2">
         <v>-90</v>
@@ -3528,10 +3568,10 @@
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="2" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="C20" s="3">
         <v>145.02000000000001</v>
@@ -3540,7 +3580,7 @@
         <v>-67.738050000000001</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="F20" s="2">
         <v>180</v>
@@ -3548,10 +3588,10 @@
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="C21" s="3">
         <v>136.28749999999999</v>
@@ -3560,7 +3600,7 @@
         <v>-131.05000000000001</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="F21" s="2">
         <v>150</v>
@@ -3568,10 +3608,10 @@
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="C22" s="3">
         <v>145.02000000000001</v>
@@ -3580,38 +3620,38 @@
         <v>-69.402050000000003</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="F22" s="2">
         <v>180</v>
       </c>
     </row>
     <row r="23" spans="1:6">
-      <c r="A23" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="C23" s="3">
+      <c r="A23" s="27" t="s">
+        <v>76</v>
+      </c>
+      <c r="B23" s="27" t="s">
+        <v>278</v>
+      </c>
+      <c r="C23" s="28">
         <v>118.7</v>
       </c>
-      <c r="D23" s="3">
+      <c r="D23" s="28">
         <v>-105.6</v>
       </c>
-      <c r="E23" s="2" t="s">
-        <v>265</v>
-      </c>
-      <c r="F23" s="2">
+      <c r="E23" s="27" t="s">
+        <v>259</v>
+      </c>
+      <c r="F23" s="27">
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="C24" s="3">
         <v>176.46497500000001</v>
@@ -3620,7 +3660,7 @@
         <v>-74.846794000000003</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="F24" s="2">
         <v>-8</v>
@@ -3628,10 +3668,10 @@
     </row>
     <row r="25" spans="1:6">
       <c r="A25" s="2" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="C25" s="3">
         <v>195.33750000000001</v>
@@ -3640,7 +3680,7 @@
         <v>-117.65</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="F25" s="2">
         <v>-15</v>
@@ -3648,10 +3688,10 @@
     </row>
     <row r="26" spans="1:6">
       <c r="A26" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="C26" s="3">
         <v>154.3425</v>
@@ -3660,7 +3700,7 @@
         <v>-68.900000000000006</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="F26" s="2">
         <v>180</v>
@@ -3668,10 +3708,10 @@
     </row>
     <row r="27" spans="1:6">
       <c r="A27" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="C27" s="3">
         <v>117.766554</v>
@@ -3680,7 +3720,7 @@
         <v>-125.52166200000001</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="F27" s="2">
         <v>-165</v>
@@ -3688,10 +3728,10 @@
     </row>
     <row r="28" spans="1:6">
       <c r="A28" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="C28" s="3">
         <v>118.80859</v>
@@ -3700,7 +3740,7 @@
         <v>-127.817234</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="F28" s="2">
         <v>-75</v>
@@ -3708,10 +3748,10 @@
     </row>
     <row r="29" spans="1:6">
       <c r="A29" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="C29" s="3">
         <v>181.5</v>
@@ -3720,7 +3760,7 @@
         <v>-91.8</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="F29" s="2">
         <v>180</v>
@@ -3728,10 +3768,10 @@
     </row>
     <row r="30" spans="1:6">
       <c r="A30" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="C30" s="3">
         <v>195.53923900000001</v>
@@ -3740,7 +3780,7 @@
         <v>-116.098782</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="F30" s="2">
         <v>165</v>
@@ -3748,10 +3788,10 @@
     </row>
     <row r="31" spans="1:6">
       <c r="A31" s="2" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="C31" s="3">
         <v>146.30000000000001</v>
@@ -3760,7 +3800,7 @@
         <v>-82.6</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="F31" s="2">
         <v>0</v>
@@ -3768,10 +3808,10 @@
     </row>
     <row r="32" spans="1:6">
       <c r="A32" s="2" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="C32" s="3">
         <v>182.693973</v>
@@ -3780,7 +3820,7 @@
         <v>-127.576626</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="F32" s="2">
         <v>-105</v>
@@ -3788,10 +3828,10 @@
     </row>
     <row r="33" spans="1:6">
       <c r="A33" s="2" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="C33" s="3">
         <v>179.12472700000001</v>
@@ -3800,7 +3840,7 @@
         <v>-130.82535200000001</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="F33" s="2">
         <v>-15</v>
@@ -3808,10 +3848,10 @@
     </row>
     <row r="34" spans="1:6">
       <c r="A34" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="C34" s="3">
         <v>209.97480400000001</v>
@@ -3820,7 +3860,7 @@
         <v>-78.738535999999996</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="F34" s="2">
         <v>-30</v>
@@ -3828,10 +3868,10 @@
     </row>
     <row r="35" spans="1:6">
       <c r="A35" s="2" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="C35" s="3">
         <v>156.54300000000001</v>
@@ -3840,7 +3880,7 @@
         <v>-67.5</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="F35" s="2">
         <v>0</v>
@@ -3848,10 +3888,10 @@
     </row>
     <row r="36" spans="1:6">
       <c r="A36" s="2" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="C36" s="3">
         <v>98.396505000000005</v>
@@ -3860,7 +3900,7 @@
         <v>-82.359247999999994</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="F36" s="2">
         <v>40</v>
@@ -3868,10 +3908,10 @@
     </row>
     <row r="37" spans="1:6">
       <c r="A37" s="2" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="C37" s="3">
         <v>119.468378</v>
@@ -3880,7 +3920,7 @@
         <v>-115.717754</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="F37" s="2">
         <v>-165</v>
@@ -3888,10 +3928,10 @@
     </row>
     <row r="38" spans="1:6">
       <c r="A38" s="2" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="C38" s="3">
         <v>104.407155</v>
@@ -3900,7 +3940,7 @@
         <v>-133.672057</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="F38" s="2">
         <v>-38</v>
@@ -3908,10 +3948,10 @@
     </row>
     <row r="39" spans="1:6">
       <c r="A39" s="2" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="C39" s="3">
         <v>137.324803</v>
@@ -3920,7 +3960,7 @@
         <v>-129.92150000000001</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="F39" s="2">
         <v>-30</v>
@@ -3928,10 +3968,10 @@
     </row>
     <row r="40" spans="1:6">
       <c r="A40" s="2" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="C40" s="3">
         <v>170.302164</v>
@@ -3940,7 +3980,7 @@
         <v>-117.65237500000001</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="F40" s="2">
         <v>144</v>
@@ -3948,10 +3988,10 @@
     </row>
     <row r="41" spans="1:6">
       <c r="A41" s="2" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="C41" s="3">
         <v>214.66533999999999</v>
@@ -3960,7 +4000,7 @@
         <v>-132.64650499999999</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="F41" s="2">
         <v>130</v>
@@ -3968,10 +4008,10 @@
     </row>
     <row r="42" spans="1:6">
       <c r="A42" s="2" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="C42" s="3">
         <v>181.596476</v>
@@ -3980,7 +4020,7 @@
         <v>-71.203723999999994</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="F42" s="2">
         <v>77</v>
@@ -3988,10 +4028,10 @@
     </row>
     <row r="43" spans="1:6">
       <c r="A43" s="2" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="C43" s="3">
         <v>132.30929599999999</v>
@@ -4000,7 +4040,7 @@
         <v>-68.084562000000005</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="F43" s="2">
         <v>-170</v>
@@ -4008,10 +4048,10 @@
     </row>
     <row r="44" spans="1:6">
       <c r="A44" s="2" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="C44" s="3">
         <v>191.97904800000001</v>
@@ -4020,7 +4060,7 @@
         <v>-71.443256000000005</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="F44" s="2">
         <v>-107</v>
@@ -4028,10 +4068,10 @@
     </row>
     <row r="45" spans="1:6">
       <c r="A45" s="2" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="C45" s="3">
         <v>144.6</v>
@@ -4040,7 +4080,7 @@
         <v>-78.400000000000006</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="F45" s="2">
         <v>90</v>
@@ -4048,10 +4088,10 @@
     </row>
     <row r="46" spans="1:6">
       <c r="A46" s="2" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="C46" s="3">
         <v>119.34344900000001</v>
@@ -4060,7 +4100,7 @@
         <v>-131.67943</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="F46" s="2">
         <v>15</v>
@@ -4068,10 +4108,10 @@
     </row>
     <row r="47" spans="1:6">
       <c r="A47" s="2" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="C47" s="3">
         <v>177.7</v>
@@ -4080,7 +4120,7 @@
         <v>-103.4</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="F47" s="2">
         <v>0</v>
@@ -4088,10 +4128,10 @@
     </row>
     <row r="48" spans="1:6">
       <c r="A48" s="2" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="C48" s="3">
         <v>81.775013999999999</v>
@@ -4100,7 +4140,7 @@
         <v>-62.336748</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="F48" s="2">
         <v>0</v>
@@ -4108,10 +4148,10 @@
     </row>
     <row r="49" spans="1:6">
       <c r="A49" s="2" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="C49" s="3">
         <v>81.95</v>
@@ -4120,7 +4160,7 @@
         <v>-62.4375</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="F49" s="2">
         <v>0</v>
@@ -4128,10 +4168,10 @@
     </row>
     <row r="50" spans="1:6">
       <c r="A50" s="2" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="C50" s="3">
         <v>187.01709700000001</v>
@@ -4140,7 +4180,7 @@
         <v>-136.50524999999999</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="F50" s="2">
         <v>165</v>
@@ -4148,10 +4188,10 @@
     </row>
     <row r="51" spans="1:6">
       <c r="A51" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C51" s="3">
         <v>148.1</v>
@@ -4160,7 +4200,7 @@
         <v>-78.900000000000006</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="F51" s="2">
         <v>180</v>
@@ -4168,10 +4208,10 @@
     </row>
     <row r="52" spans="1:6">
       <c r="A52" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="C52" s="3">
         <v>157.36291399999999</v>
@@ -4180,7 +4220,7 @@
         <v>-70.990414000000001</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="F52" s="2">
         <v>-8</v>
@@ -4188,10 +4228,10 @@
     </row>
     <row r="53" spans="1:6">
       <c r="A53" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="C53" s="3">
         <v>218.895882</v>
@@ -4200,7 +4240,7 @@
         <v>-92.596930999999998</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="F53" s="2">
         <v>-80</v>
@@ -4208,10 +4248,10 @@
     </row>
     <row r="54" spans="1:6">
       <c r="A54" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="C54" s="3">
         <v>199.406702</v>
@@ -4220,7 +4260,7 @@
         <v>-96.374824000000004</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="F54" s="2">
         <v>-80</v>
@@ -4228,10 +4268,10 @@
     </row>
     <row r="55" spans="1:6">
       <c r="A55" s="2" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="C55" s="3">
         <v>198.31601599999999</v>
@@ -4240,7 +4280,7 @@
         <v>-110.221113</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="F55" s="2">
         <v>-74</v>
@@ -4248,10 +4288,10 @@
     </row>
     <row r="56" spans="1:6">
       <c r="A56" s="2" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="C56" s="3">
         <v>188.21676099999999</v>
@@ -4260,7 +4300,7 @@
         <v>-128.148248</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="F56" s="2">
         <v>-105</v>
@@ -4268,10 +4308,10 @@
     </row>
     <row r="57" spans="1:6">
       <c r="A57" s="2" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="C57" s="3">
         <v>190.14861099999999</v>
@@ -4280,7 +4320,7 @@
         <v>-128.665886</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="F57" s="2">
         <v>-105</v>
@@ -4288,10 +4328,10 @@
     </row>
     <row r="58" spans="1:6">
       <c r="A58" s="2" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="C58" s="3">
         <v>202.525825</v>
@@ -4300,7 +4340,7 @@
         <v>-116.490077</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="F58" s="2">
         <v>-39</v>
@@ -4308,10 +4348,10 @@
     </row>
     <row r="59" spans="1:6">
       <c r="A59" s="2" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="C59" s="3">
         <v>225.235221</v>
@@ -4320,7 +4360,7 @@
         <v>-107.529645</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="F59" s="2">
         <v>-90</v>
@@ -4328,10 +4368,10 @@
     </row>
     <row r="60" spans="1:6">
       <c r="A60" s="2" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="C60" s="3">
         <v>197.567666</v>
@@ -4340,7 +4380,7 @@
         <v>-102.203459</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="F60" s="2">
         <v>-15</v>
@@ -4348,10 +4388,10 @@
     </row>
     <row r="61" spans="1:6">
       <c r="A61" s="2" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="C61" s="3">
         <v>141.65</v>
@@ -4360,7 +4400,7 @@
         <v>-117.62</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="F61" s="2">
         <v>0</v>
@@ -4368,10 +4408,10 @@
     </row>
     <row r="62" spans="1:6">
       <c r="A62" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="C62" s="3">
         <v>175.25</v>
@@ -4380,7 +4420,7 @@
         <v>-91.8</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="F62" s="2">
         <v>180</v>
@@ -4388,10 +4428,10 @@
     </row>
     <row r="63" spans="1:6">
       <c r="A63" s="2" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="C63" s="3">
         <v>123.53743299999999</v>
@@ -4400,7 +4440,7 @@
         <v>-130.44537099999999</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="F63" s="2">
         <v>105</v>
@@ -4408,10 +4448,10 @@
     </row>
     <row r="64" spans="1:6">
       <c r="A64" s="2" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="C64" s="3">
         <v>124.759731</v>
@@ -4420,7 +4460,7 @@
         <v>-128.89282600000001</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="F64" s="2">
         <v>105</v>
@@ -4428,10 +4468,10 @@
     </row>
     <row r="65" spans="1:6">
       <c r="A65" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="C65" s="3">
         <v>123.827997</v>
@@ -4440,7 +4480,7 @@
         <v>-125.945494</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="F65" s="2">
         <v>105</v>
@@ -4448,10 +4488,10 @@
     </row>
     <row r="66" spans="1:6">
       <c r="A66" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="C66" s="3">
         <v>120.776233</v>
@@ -4460,7 +4500,7 @@
         <v>-124.728162</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="F66" s="2">
         <v>-165</v>
@@ -4468,10 +4508,10 @@
     </row>
     <row r="67" spans="1:6">
       <c r="A67" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="C67" s="3">
         <v>140.44399999999999</v>
@@ -4480,7 +4520,7 @@
         <v>-77.650000000000006</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="F67" s="2">
         <v>-90</v>
@@ -4488,10 +4528,10 @@
     </row>
     <row r="68" spans="1:6">
       <c r="A68" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="C68" s="3">
         <v>186.284909</v>
@@ -4500,7 +4540,7 @@
         <v>-127.63061</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="F68" s="2">
         <v>-105</v>
@@ -4508,10 +4548,10 @@
     </row>
     <row r="69" spans="1:6">
       <c r="A69" s="2" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="C69" s="3">
         <v>192.08046400000001</v>
@@ -4520,7 +4560,7 @@
         <v>-129.183525</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="F69" s="2">
         <v>-105</v>
@@ -4528,10 +4568,10 @@
     </row>
     <row r="70" spans="1:6">
       <c r="A70" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="C70" s="3">
         <v>178.4</v>
@@ -4540,7 +4580,7 @@
         <v>-91.8</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="F70" s="2">
         <v>0</v>
@@ -4548,10 +4588,10 @@
     </row>
     <row r="71" spans="1:6">
       <c r="A71" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="C71" s="3">
         <v>193.55</v>
@@ -4560,7 +4600,7 @@
         <v>-113.0625</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="F71" s="2">
         <v>90</v>
@@ -4568,10 +4608,10 @@
     </row>
     <row r="72" spans="1:6">
       <c r="A72" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="C72" s="3">
         <v>136.17449999999999</v>
@@ -4580,7 +4620,7 @@
         <v>-85.59</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="F72" s="2">
         <v>0</v>
@@ -4588,10 +4628,10 @@
     </row>
     <row r="73" spans="1:6">
       <c r="A73" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="C73" s="3">
         <v>145.15</v>
@@ -4600,7 +4640,7 @@
         <v>-117.62</v>
       </c>
       <c r="E73" s="2" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="F73" s="2">
         <v>0</v>
@@ -4608,10 +4648,10 @@
     </row>
     <row r="74" spans="1:6">
       <c r="A74" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="C74" s="3">
         <v>150.69999999999999</v>
@@ -4620,7 +4660,7 @@
         <v>-78.900000000000006</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="F74" s="2">
         <v>90</v>
@@ -4628,10 +4668,10 @@
     </row>
     <row r="75" spans="1:6">
       <c r="A75" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="C75" s="3">
         <v>136.94999999999999</v>
@@ -4640,7 +4680,7 @@
         <v>-124.7</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="F75" s="2">
         <v>180</v>
@@ -4648,10 +4688,10 @@
     </row>
     <row r="76" spans="1:6">
       <c r="A76" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="C76" s="3">
         <v>139.30000000000001</v>
@@ -4660,7 +4700,7 @@
         <v>-91.05</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="F76" s="2">
         <v>180</v>
@@ -4668,10 +4708,10 @@
     </row>
     <row r="77" spans="1:6">
       <c r="A77" s="2" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="C77" s="3">
         <v>118.866524</v>
@@ -4680,7 +4720,7 @@
         <v>-73.302024000000003</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="F77" s="2">
         <v>-152</v>
@@ -4688,10 +4728,10 @@
     </row>
     <row r="78" spans="1:6">
       <c r="A78" s="2" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="C78" s="3">
         <v>105.79314599999999</v>
@@ -4700,7 +4740,7 @@
         <v>-91.593145000000007</v>
       </c>
       <c r="E78" s="2" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="F78" s="2">
         <v>-45</v>
@@ -4708,10 +4748,10 @@
     </row>
     <row r="79" spans="1:6">
       <c r="A79" s="2" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="C79" s="3">
         <v>111.45</v>
@@ -4720,7 +4760,7 @@
         <v>-97.25</v>
       </c>
       <c r="E79" s="2" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="F79" s="2">
         <v>-135</v>
@@ -4728,10 +4768,10 @@
     </row>
     <row r="80" spans="1:6">
       <c r="A80" s="2" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="C80" s="3">
         <v>100.136291</v>
@@ -4740,7 +4780,7 @@
         <v>-97.25</v>
       </c>
       <c r="E80" s="2" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="F80" s="2">
         <v>45</v>
@@ -4748,10 +4788,10 @@
     </row>
     <row r="81" spans="1:6">
       <c r="A81" s="2" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="C81" s="3">
         <v>105.79314599999999</v>
@@ -4760,7 +4800,7 @@
         <v>-102.906854</v>
       </c>
       <c r="E81" s="2" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="F81" s="2">
         <v>135</v>
@@ -4768,10 +4808,10 @@
     </row>
     <row r="82" spans="1:6">
       <c r="A82" s="2" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="C82" s="3">
         <v>123.071451</v>
@@ -4780,7 +4820,7 @@
         <v>-108.76933200000001</v>
       </c>
       <c r="E82" s="2" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="F82" s="2">
         <v>-170</v>
@@ -4788,10 +4828,10 @@
     </row>
     <row r="83" spans="1:6">
       <c r="A83" s="2" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="C83" s="3">
         <v>121.835076</v>
@@ -4800,7 +4840,7 @@
         <v>-101.757501</v>
       </c>
       <c r="E83" s="2" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="F83" s="2">
         <v>-170</v>
@@ -4808,10 +4848,10 @@
     </row>
     <row r="84" spans="1:6">
       <c r="A84" s="2" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="C84" s="3">
         <v>183.519015</v>
@@ -4820,7 +4860,7 @@
         <v>-91.518992999999995</v>
       </c>
       <c r="E84" s="2" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="F84" s="2">
         <v>110</v>
@@ -4828,10 +4868,10 @@
     </row>
     <row r="85" spans="1:6">
       <c r="A85" s="2" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="C85" s="3">
         <v>195.11901499999999</v>
@@ -4840,7 +4880,7 @@
         <v>-85.968992999999998</v>
       </c>
       <c r="E85" s="2" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="F85" s="2">
         <v>110</v>
@@ -4848,10 +4888,10 @@
     </row>
     <row r="86" spans="1:6">
       <c r="A86" s="2" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="C86" s="3">
         <v>123.168148</v>
@@ -4860,7 +4900,7 @@
         <v>-134.76763800000001</v>
       </c>
       <c r="E86" s="2" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="F86" s="2">
         <v>-165</v>
@@ -4868,10 +4908,10 @@
     </row>
     <row r="87" spans="1:6">
       <c r="A87" s="2" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="C87" s="3">
         <v>166.34687500000001</v>
@@ -4880,7 +4920,7 @@
         <v>-77.070689000000002</v>
       </c>
       <c r="E87" s="2" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="F87" s="2">
         <v>172</v>
@@ -4888,10 +4928,10 @@
     </row>
     <row r="88" spans="1:6">
       <c r="A88" s="2" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="C88" s="3">
         <v>147.88</v>
@@ -4900,7 +4940,7 @@
         <v>-124.5</v>
       </c>
       <c r="E88" s="2" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="F88" s="2">
         <v>180</v>
@@ -4908,10 +4948,10 @@
     </row>
     <row r="89" spans="1:6">
       <c r="A89" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="C89" s="3">
         <v>69.033475999999993</v>
@@ -4920,7 +4960,7 @@
         <v>-217.44825</v>
       </c>
       <c r="E89" s="2" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="F89" s="2">
         <v>0</v>
@@ -4928,10 +4968,10 @@
     </row>
     <row r="90" spans="1:6">
       <c r="A90" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="C90" s="3">
         <v>121.46060199999999</v>
@@ -4940,7 +4980,7 @@
         <v>-127.37885300000001</v>
       </c>
       <c r="E90" s="2" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="F90" s="2">
         <v>105</v>
@@ -4948,10 +4988,10 @@
     </row>
     <row r="91" spans="1:6">
       <c r="A91" s="2" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="C91" s="3">
         <v>142.30000000000001</v>
@@ -4960,7 +5000,7 @@
         <v>-70.91</v>
       </c>
       <c r="E91" s="2" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="F91" s="2">
         <v>0</v>
@@ -4968,10 +5008,10 @@
     </row>
     <row r="92" spans="1:6">
       <c r="A92" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="C92" s="3">
         <v>140.32400000000001</v>
@@ -4980,7 +5020,7 @@
         <v>-122.2735</v>
       </c>
       <c r="E92" s="2" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="F92" s="2">
         <v>180</v>
@@ -4988,10 +5028,10 @@
     </row>
     <row r="93" spans="1:6">
       <c r="A93" s="2" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C93" s="3">
         <v>150.04599999999999</v>
@@ -5000,7 +5040,7 @@
         <v>-68.468000000000004</v>
       </c>
       <c r="E93" s="2" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="F93" s="2">
         <v>0</v>
@@ -5008,10 +5048,10 @@
     </row>
     <row r="94" spans="1:6">
       <c r="A94" s="2" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="C94" s="3">
         <v>133.98099999999999</v>
@@ -5020,7 +5060,7 @@
         <v>-89.099000000000004</v>
       </c>
       <c r="E94" s="2" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="F94" s="2">
         <v>180</v>
@@ -5028,10 +5068,10 @@
     </row>
     <row r="95" spans="1:6">
       <c r="A95" s="2" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="C95" s="3">
         <v>123.05685200000001</v>
@@ -5040,7 +5080,7 @@
         <v>-85.588319999999996</v>
       </c>
       <c r="E95" s="2" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="F95" s="2">
         <v>-3</v>

</xml_diff>

<commit_message>
quoting data to prepare for order
</commit_message>
<xml_diff>
--- a/Swadge-HW/Manufacturing Information/Hot Dog Quotation.xlsx
+++ b/Swadge-HW/Manufacturing Information/Hot Dog Quotation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eanthony\Documents\GitHub\Super-2025-Swadge-HW\Swadge-HW\Manufacturing Information\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7B9EACE-13D5-49A0-8AE8-2E58CB330D8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8A6FB49-D472-4184-8FEA-72B48D259028}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PCB Specification" sheetId="5" r:id="rId1"/>
@@ -1168,7 +1168,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1224,18 +1224,6 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1251,6 +1239,21 @@
     </xf>
     <xf numFmtId="3" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -1657,8 +1660,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1671,14 +1674,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19" t="s">
+      <c r="B1" s="25"/>
+      <c r="C1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="19"/>
+      <c r="D1" s="25"/>
       <c r="E1" s="1"/>
     </row>
     <row r="2" spans="1:5">
@@ -1839,22 +1842,22 @@
       <c r="E12" s="1"/>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="20" t="s">
+      <c r="A13" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="20"/>
-      <c r="C13" s="20"/>
-      <c r="D13" s="20"/>
-      <c r="E13" s="20"/>
+      <c r="B13" s="26"/>
+      <c r="C13" s="26"/>
+      <c r="D13" s="26"/>
+      <c r="E13" s="26"/>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="21" t="s">
+      <c r="A14" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="20"/>
-      <c r="C14" s="20"/>
-      <c r="D14" s="20"/>
-      <c r="E14" s="20"/>
+      <c r="B14" s="26"/>
+      <c r="C14" s="26"/>
+      <c r="D14" s="26"/>
+      <c r="E14" s="26"/>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="1"/>
@@ -1863,25 +1866,33 @@
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
     </row>
-    <row r="18" spans="2:2">
-      <c r="B18" t="s">
+    <row r="18" spans="2:4">
+      <c r="B18" s="29" t="s">
         <v>273</v>
       </c>
-    </row>
-    <row r="19" spans="2:2">
-      <c r="B19" t="s">
+      <c r="C18" s="29"/>
+      <c r="D18" s="29"/>
+    </row>
+    <row r="19" spans="2:4">
+      <c r="B19" s="29" t="s">
         <v>274</v>
       </c>
-    </row>
-    <row r="20" spans="2:2">
-      <c r="B20" t="s">
+      <c r="C19" s="29"/>
+      <c r="D19" s="29"/>
+    </row>
+    <row r="20" spans="2:4">
+      <c r="B20" s="29" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="21" spans="2:2">
-      <c r="B21" t="s">
+      <c r="C20" s="29"/>
+      <c r="D20" s="29"/>
+    </row>
+    <row r="21" spans="2:4">
+      <c r="B21" s="29" t="s">
         <v>276</v>
       </c>
+      <c r="C21" s="29"/>
+      <c r="D21" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1919,20 +1930,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="4" customFormat="1" ht="26.25">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
-      <c r="L1" s="22"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="28"/>
     </row>
     <row r="2" spans="1:12" s="4" customFormat="1" ht="14.25">
       <c r="A2" s="5" t="s">
@@ -2141,33 +2152,33 @@
       </c>
       <c r="L8" s="15"/>
     </row>
-    <row r="9" spans="1:12" s="26" customFormat="1">
-      <c r="A9" s="23">
+    <row r="9" spans="1:12" s="22" customFormat="1">
+      <c r="A9" s="19">
         <v>7</v>
       </c>
-      <c r="B9" s="24" t="s">
+      <c r="B9" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="C9" s="24">
+      <c r="C9" s="20">
         <v>1</v>
       </c>
-      <c r="D9" s="24" t="s">
+      <c r="D9" s="20" t="s">
         <v>277</v>
       </c>
-      <c r="E9" s="25" t="s">
+      <c r="E9" s="21" t="s">
         <v>278</v>
       </c>
-      <c r="F9" s="24"/>
-      <c r="H9" s="24">
+      <c r="F9" s="20"/>
+      <c r="H9" s="20">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="I9" s="23"/>
-      <c r="J9" s="23"/>
-      <c r="K9" s="24" t="s">
+      <c r="I9" s="19"/>
+      <c r="J9" s="19"/>
+      <c r="K9" s="20" t="s">
         <v>268</v>
       </c>
-      <c r="L9" s="24"/>
+      <c r="L9" s="20"/>
     </row>
     <row r="10" spans="1:12" s="4" customFormat="1">
       <c r="A10" s="5">
@@ -3143,7 +3154,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B2:B35"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="T31" sqref="T31"/>
     </sheetView>
   </sheetViews>
@@ -3171,7 +3182,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F178"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
@@ -3627,22 +3638,22 @@
       </c>
     </row>
     <row r="23" spans="1:6">
-      <c r="A23" s="27" t="s">
+      <c r="A23" s="23" t="s">
         <v>76</v>
       </c>
-      <c r="B23" s="27" t="s">
+      <c r="B23" s="23" t="s">
         <v>278</v>
       </c>
-      <c r="C23" s="28">
+      <c r="C23" s="24">
         <v>118.7</v>
       </c>
-      <c r="D23" s="28">
+      <c r="D23" s="24">
         <v>-105.6</v>
       </c>
-      <c r="E23" s="27" t="s">
-        <v>259</v>
-      </c>
-      <c r="F23" s="27">
+      <c r="E23" s="23" t="s">
+        <v>259</v>
+      </c>
+      <c r="F23" s="23">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Rev 0 for release
</commit_message>
<xml_diff>
--- a/Swadge-HW/Manufacturing Information/Hot Dog Quotation.xlsx
+++ b/Swadge-HW/Manufacturing Information/Hot Dog Quotation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eanthony\Documents\GitHub\Super-2025-Swadge-HW\Swadge-HW\Manufacturing Information\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8A6FB49-D472-4184-8FEA-72B48D259028}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43343518-877F-47AD-932A-68DFF13E455F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="279">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="275">
   <si>
     <t>Your PCB Specification</t>
   </si>
@@ -910,18 +910,6 @@
   </si>
   <si>
     <t>rotation</t>
-  </si>
-  <si>
-    <t>N1</t>
-  </si>
-  <si>
-    <t>N2</t>
-  </si>
-  <si>
-    <t>hotdog-outline</t>
-  </si>
-  <si>
-    <t>condiment</t>
   </si>
   <si>
     <t>layer</t>
@@ -1240,6 +1228,9 @@
     <xf numFmtId="3" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1251,9 +1242,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -1661,7 +1649,7 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1674,14 +1662,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25" t="s">
+      <c r="B1" s="26"/>
+      <c r="C1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="25"/>
+      <c r="D1" s="26"/>
       <c r="E1" s="1"/>
     </row>
     <row r="2" spans="1:5">
@@ -1689,13 +1677,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>1</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="E2" s="1"/>
     </row>
@@ -1779,13 +1767,13 @@
         <v>11</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="C8" s="10" t="s">
         <v>11</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="E8" s="1"/>
     </row>
@@ -1842,22 +1830,22 @@
       <c r="E12" s="1"/>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="26" t="s">
+      <c r="A13" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="26"/>
-      <c r="C13" s="26"/>
-      <c r="D13" s="26"/>
-      <c r="E13" s="26"/>
+      <c r="B13" s="27"/>
+      <c r="C13" s="27"/>
+      <c r="D13" s="27"/>
+      <c r="E13" s="27"/>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="27" t="s">
+      <c r="A14" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="26"/>
-      <c r="C14" s="26"/>
-      <c r="D14" s="26"/>
-      <c r="E14" s="26"/>
+      <c r="B14" s="27"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="27"/>
+      <c r="E14" s="27"/>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="1"/>
@@ -1867,32 +1855,32 @@
       <c r="E15" s="1"/>
     </row>
     <row r="18" spans="2:4">
-      <c r="B18" s="29" t="s">
-        <v>273</v>
-      </c>
-      <c r="C18" s="29"/>
-      <c r="D18" s="29"/>
+      <c r="B18" s="25" t="s">
+        <v>269</v>
+      </c>
+      <c r="C18" s="25"/>
+      <c r="D18" s="25"/>
     </row>
     <row r="19" spans="2:4">
-      <c r="B19" s="29" t="s">
-        <v>274</v>
-      </c>
-      <c r="C19" s="29"/>
-      <c r="D19" s="29"/>
+      <c r="B19" s="25" t="s">
+        <v>270</v>
+      </c>
+      <c r="C19" s="25"/>
+      <c r="D19" s="25"/>
     </row>
     <row r="20" spans="2:4">
-      <c r="B20" s="29" t="s">
-        <v>275</v>
-      </c>
-      <c r="C20" s="29"/>
-      <c r="D20" s="29"/>
+      <c r="B20" s="25" t="s">
+        <v>271</v>
+      </c>
+      <c r="C20" s="25"/>
+      <c r="D20" s="25"/>
     </row>
     <row r="21" spans="2:4">
-      <c r="B21" s="29" t="s">
-        <v>276</v>
-      </c>
-      <c r="C21" s="29"/>
-      <c r="D21" s="29"/>
+      <c r="B21" s="25" t="s">
+        <v>272</v>
+      </c>
+      <c r="C21" s="25"/>
+      <c r="D21" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1930,20 +1918,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="4" customFormat="1" ht="26.25">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
-      <c r="K1" s="28"/>
-      <c r="L1" s="28"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
+      <c r="K1" s="29"/>
+      <c r="L1" s="29"/>
     </row>
     <row r="2" spans="1:12" s="4" customFormat="1" ht="14.25">
       <c r="A2" s="5" t="s">
@@ -2148,7 +2136,7 @@
       <c r="I8" s="5"/>
       <c r="J8" s="5"/>
       <c r="K8" s="15" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="L8" s="15"/>
     </row>
@@ -2163,10 +2151,10 @@
         <v>1</v>
       </c>
       <c r="D9" s="20" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="E9" s="21" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="F9" s="20"/>
       <c r="H9" s="20">
@@ -2176,7 +2164,7 @@
       <c r="I9" s="19"/>
       <c r="J9" s="19"/>
       <c r="K9" s="20" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="L9" s="20"/>
     </row>
@@ -2887,7 +2875,7 @@
         <v>154</v>
       </c>
       <c r="F34" s="15" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="I34" s="15">
         <f>C34</f>
@@ -3167,7 +3155,7 @@
     </row>
     <row r="35" spans="2:2">
       <c r="B35" s="18" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
     </row>
   </sheetData>
@@ -3180,10 +3168,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:F178"/>
+  <dimension ref="A1:F176"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+    <sheetView topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="H98" sqref="H98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -3211,7 +3199,7 @@
         <v>258</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>260</v>
@@ -3225,10 +3213,10 @@
         <v>2460</v>
       </c>
       <c r="C2" s="3">
-        <v>211.806016</v>
+        <v>211.80600000000001</v>
       </c>
       <c r="D2" s="3">
-        <v>-110.399922</v>
+        <v>-110.3999</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>259</v>
@@ -3265,10 +3253,10 @@
         <v>2460</v>
       </c>
       <c r="C4" s="3">
-        <v>103.313985</v>
+        <v>103.31399999999999</v>
       </c>
       <c r="D4" s="3">
-        <v>-107.749922</v>
+        <v>-107.7499</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>259</v>
@@ -3285,10 +3273,10 @@
         <v>140</v>
       </c>
       <c r="C5" s="3">
-        <v>157.64126099999999</v>
+        <v>157.6413</v>
       </c>
       <c r="D5" s="3">
-        <v>-69.009878</v>
+        <v>-69.009900000000002</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>259</v>
@@ -3505,10 +3493,10 @@
         <v>140</v>
       </c>
       <c r="C16" s="3">
-        <v>176.68152900000001</v>
+        <v>176.6815</v>
       </c>
       <c r="D16" s="3">
-        <v>-73.305937</v>
+        <v>-73.305899999999994</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>259</v>
@@ -3588,7 +3576,7 @@
         <v>145.02000000000001</v>
       </c>
       <c r="D20" s="3">
-        <v>-67.738050000000001</v>
+        <v>-67.738100000000003</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>259</v>
@@ -3628,7 +3616,7 @@
         <v>145.02000000000001</v>
       </c>
       <c r="D22" s="3">
-        <v>-69.402050000000003</v>
+        <v>-69.402100000000004</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>259</v>
@@ -3642,7 +3630,7 @@
         <v>76</v>
       </c>
       <c r="B23" s="23" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="C23" s="24">
         <v>118.7</v>
@@ -3665,10 +3653,10 @@
         <v>140</v>
       </c>
       <c r="C24" s="3">
-        <v>176.46497500000001</v>
+        <v>176.465</v>
       </c>
       <c r="D24" s="3">
-        <v>-74.846794000000003</v>
+        <v>-74.846800000000002</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>259</v>
@@ -3725,10 +3713,10 @@
         <v>140</v>
       </c>
       <c r="C27" s="3">
-        <v>117.766554</v>
+        <v>117.7666</v>
       </c>
       <c r="D27" s="3">
-        <v>-125.52166200000001</v>
+        <v>-125.5217</v>
       </c>
       <c r="E27" s="2" t="s">
         <v>259</v>
@@ -3745,10 +3733,10 @@
         <v>140</v>
       </c>
       <c r="C28" s="3">
-        <v>118.80859</v>
+        <v>118.8086</v>
       </c>
       <c r="D28" s="3">
-        <v>-127.817234</v>
+        <v>-127.8172</v>
       </c>
       <c r="E28" s="2" t="s">
         <v>259</v>
@@ -3785,10 +3773,10 @@
         <v>141</v>
       </c>
       <c r="C30" s="3">
-        <v>195.53923900000001</v>
+        <v>195.53919999999999</v>
       </c>
       <c r="D30" s="3">
-        <v>-116.098782</v>
+        <v>-116.0988</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>212</v>
@@ -3825,10 +3813,10 @@
         <v>143</v>
       </c>
       <c r="C32" s="3">
-        <v>182.693973</v>
+        <v>182.69399999999999</v>
       </c>
       <c r="D32" s="3">
-        <v>-127.576626</v>
+        <v>-127.5766</v>
       </c>
       <c r="E32" s="2" t="s">
         <v>259</v>
@@ -3845,10 +3833,10 @@
         <v>142</v>
       </c>
       <c r="C33" s="3">
-        <v>179.12472700000001</v>
+        <v>179.12469999999999</v>
       </c>
       <c r="D33" s="3">
-        <v>-130.82535200000001</v>
+        <v>-130.8254</v>
       </c>
       <c r="E33" s="2" t="s">
         <v>259</v>
@@ -3865,10 +3853,10 @@
         <v>141</v>
       </c>
       <c r="C34" s="3">
-        <v>209.97480400000001</v>
+        <v>209.97479999999999</v>
       </c>
       <c r="D34" s="3">
-        <v>-78.738535999999996</v>
+        <v>-78.738500000000002</v>
       </c>
       <c r="E34" s="2" t="s">
         <v>212</v>
@@ -3905,10 +3893,10 @@
         <v>141</v>
       </c>
       <c r="C36" s="3">
-        <v>98.396505000000005</v>
+        <v>98.396500000000003</v>
       </c>
       <c r="D36" s="3">
-        <v>-82.359247999999994</v>
+        <v>-82.359200000000001</v>
       </c>
       <c r="E36" s="2" t="s">
         <v>212</v>
@@ -3925,10 +3913,10 @@
         <v>141</v>
       </c>
       <c r="C37" s="3">
-        <v>119.468378</v>
+        <v>119.4684</v>
       </c>
       <c r="D37" s="3">
-        <v>-115.717754</v>
+        <v>-115.7178</v>
       </c>
       <c r="E37" s="2" t="s">
         <v>212</v>
@@ -3945,10 +3933,10 @@
         <v>141</v>
       </c>
       <c r="C38" s="3">
-        <v>104.407155</v>
+        <v>104.4072</v>
       </c>
       <c r="D38" s="3">
-        <v>-133.672057</v>
+        <v>-133.6721</v>
       </c>
       <c r="E38" s="2" t="s">
         <v>212</v>
@@ -3965,7 +3953,7 @@
         <v>141</v>
       </c>
       <c r="C39" s="3">
-        <v>137.324803</v>
+        <v>137.32480000000001</v>
       </c>
       <c r="D39" s="3">
         <v>-129.92150000000001</v>
@@ -3985,10 +3973,10 @@
         <v>141</v>
       </c>
       <c r="C40" s="3">
-        <v>170.302164</v>
+        <v>170.3022</v>
       </c>
       <c r="D40" s="3">
-        <v>-117.65237500000001</v>
+        <v>-117.6524</v>
       </c>
       <c r="E40" s="2" t="s">
         <v>212</v>
@@ -4005,10 +3993,10 @@
         <v>141</v>
       </c>
       <c r="C41" s="3">
-        <v>214.66533999999999</v>
+        <v>214.6653</v>
       </c>
       <c r="D41" s="3">
-        <v>-132.64650499999999</v>
+        <v>-132.6465</v>
       </c>
       <c r="E41" s="2" t="s">
         <v>212</v>
@@ -4025,10 +4013,10 @@
         <v>144</v>
       </c>
       <c r="C42" s="3">
-        <v>181.596476</v>
+        <v>181.59649999999999</v>
       </c>
       <c r="D42" s="3">
-        <v>-71.203723999999994</v>
+        <v>-71.203699999999998</v>
       </c>
       <c r="E42" s="2" t="s">
         <v>212</v>
@@ -4045,10 +4033,10 @@
         <v>114</v>
       </c>
       <c r="C43" s="3">
-        <v>132.30929599999999</v>
+        <v>132.30930000000001</v>
       </c>
       <c r="D43" s="3">
-        <v>-68.084562000000005</v>
+        <v>-68.084599999999995</v>
       </c>
       <c r="E43" s="2" t="s">
         <v>259</v>
@@ -4065,10 +4053,10 @@
         <v>256</v>
       </c>
       <c r="C44" s="3">
-        <v>191.97904800000001</v>
+        <v>191.97900000000001</v>
       </c>
       <c r="D44" s="3">
-        <v>-71.443256000000005</v>
+        <v>-71.443299999999994</v>
       </c>
       <c r="E44" s="2" t="s">
         <v>259</v>
@@ -4105,10 +4093,10 @@
         <v>146</v>
       </c>
       <c r="C46" s="3">
-        <v>119.34344900000001</v>
+        <v>119.3434</v>
       </c>
       <c r="D46" s="3">
-        <v>-131.67943</v>
+        <v>-131.67939999999999</v>
       </c>
       <c r="E46" s="2" t="s">
         <v>259</v>
@@ -4139,316 +4127,316 @@
     </row>
     <row r="48" spans="1:6">
       <c r="A48" s="2" t="s">
-        <v>261</v>
+        <v>85</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>263</v>
+        <v>148</v>
       </c>
       <c r="C48" s="3">
-        <v>81.775013999999999</v>
+        <v>187.0171</v>
       </c>
       <c r="D48" s="3">
-        <v>-62.336748</v>
+        <v>-136.5052</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>212</v>
+        <v>259</v>
       </c>
       <c r="F48" s="2">
-        <v>0</v>
+        <v>165</v>
       </c>
     </row>
     <row r="49" spans="1:6">
       <c r="A49" s="2" t="s">
-        <v>262</v>
+        <v>58</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>264</v>
+        <v>35</v>
       </c>
       <c r="C49" s="3">
-        <v>81.95</v>
+        <v>148.1</v>
       </c>
       <c r="D49" s="3">
-        <v>-62.4375</v>
+        <v>-78.900000000000006</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>212</v>
+        <v>259</v>
       </c>
       <c r="F49" s="2">
-        <v>0</v>
+        <v>180</v>
       </c>
     </row>
     <row r="50" spans="1:6">
       <c r="A50" s="2" t="s">
-        <v>85</v>
+        <v>57</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C50" s="3">
-        <v>187.01709700000001</v>
+        <v>157.3629</v>
       </c>
       <c r="D50" s="3">
-        <v>-136.50524999999999</v>
+        <v>-70.990399999999994</v>
       </c>
       <c r="E50" s="2" t="s">
         <v>259</v>
       </c>
       <c r="F50" s="2">
-        <v>165</v>
+        <v>-8</v>
       </c>
     </row>
     <row r="51" spans="1:6">
       <c r="A51" s="2" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>35</v>
+        <v>149</v>
       </c>
       <c r="C51" s="3">
-        <v>148.1</v>
+        <v>218.89590000000001</v>
       </c>
       <c r="D51" s="3">
-        <v>-78.900000000000006</v>
+        <v>-92.596900000000005</v>
       </c>
       <c r="E51" s="2" t="s">
         <v>259</v>
       </c>
       <c r="F51" s="2">
-        <v>180</v>
+        <v>-80</v>
       </c>
     </row>
     <row r="52" spans="1:6">
       <c r="A52" s="2" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="B52" s="2" t="s">
         <v>149</v>
       </c>
       <c r="C52" s="3">
-        <v>157.36291399999999</v>
+        <v>199.4067</v>
       </c>
       <c r="D52" s="3">
-        <v>-70.990414000000001</v>
+        <v>-96.374799999999993</v>
       </c>
       <c r="E52" s="2" t="s">
         <v>259</v>
       </c>
       <c r="F52" s="2">
-        <v>-8</v>
+        <v>-80</v>
       </c>
     </row>
     <row r="53" spans="1:6">
       <c r="A53" s="2" t="s">
-        <v>50</v>
+        <v>245</v>
       </c>
       <c r="B53" s="2" t="s">
         <v>149</v>
       </c>
       <c r="C53" s="3">
-        <v>218.895882</v>
+        <v>198.316</v>
       </c>
       <c r="D53" s="3">
-        <v>-92.596930999999998</v>
+        <v>-110.22110000000001</v>
       </c>
       <c r="E53" s="2" t="s">
         <v>259</v>
       </c>
       <c r="F53" s="2">
-        <v>-80</v>
+        <v>-74</v>
       </c>
     </row>
     <row r="54" spans="1:6">
       <c r="A54" s="2" t="s">
-        <v>49</v>
+        <v>246</v>
       </c>
       <c r="B54" s="2" t="s">
         <v>149</v>
       </c>
       <c r="C54" s="3">
-        <v>199.406702</v>
+        <v>188.21680000000001</v>
       </c>
       <c r="D54" s="3">
-        <v>-96.374824000000004</v>
+        <v>-128.1482</v>
       </c>
       <c r="E54" s="2" t="s">
         <v>259</v>
       </c>
       <c r="F54" s="2">
-        <v>-80</v>
+        <v>-105</v>
       </c>
     </row>
     <row r="55" spans="1:6">
       <c r="A55" s="2" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="B55" s="2" t="s">
         <v>149</v>
       </c>
       <c r="C55" s="3">
-        <v>198.31601599999999</v>
+        <v>190.14859999999999</v>
       </c>
       <c r="D55" s="3">
-        <v>-110.221113</v>
+        <v>-128.66589999999999</v>
       </c>
       <c r="E55" s="2" t="s">
         <v>259</v>
       </c>
       <c r="F55" s="2">
-        <v>-74</v>
+        <v>-105</v>
       </c>
     </row>
     <row r="56" spans="1:6">
       <c r="A56" s="2" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="B56" s="2" t="s">
         <v>149</v>
       </c>
       <c r="C56" s="3">
-        <v>188.21676099999999</v>
+        <v>202.5258</v>
       </c>
       <c r="D56" s="3">
-        <v>-128.148248</v>
+        <v>-116.4901</v>
       </c>
       <c r="E56" s="2" t="s">
         <v>259</v>
       </c>
       <c r="F56" s="2">
-        <v>-105</v>
+        <v>-39</v>
       </c>
     </row>
     <row r="57" spans="1:6">
       <c r="A57" s="2" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="B57" s="2" t="s">
         <v>149</v>
       </c>
       <c r="C57" s="3">
-        <v>190.14861099999999</v>
+        <v>225.23519999999999</v>
       </c>
       <c r="D57" s="3">
-        <v>-128.665886</v>
+        <v>-107.5296</v>
       </c>
       <c r="E57" s="2" t="s">
         <v>259</v>
       </c>
       <c r="F57" s="2">
-        <v>-105</v>
+        <v>-90</v>
       </c>
     </row>
     <row r="58" spans="1:6">
       <c r="A58" s="2" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="B58" s="2" t="s">
         <v>149</v>
       </c>
       <c r="C58" s="3">
-        <v>202.525825</v>
+        <v>197.5677</v>
       </c>
       <c r="D58" s="3">
-        <v>-116.490077</v>
+        <v>-102.20350000000001</v>
       </c>
       <c r="E58" s="2" t="s">
         <v>259</v>
       </c>
       <c r="F58" s="2">
-        <v>-39</v>
+        <v>-15</v>
       </c>
     </row>
     <row r="59" spans="1:6">
       <c r="A59" s="2" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="B59" s="2" t="s">
         <v>149</v>
       </c>
       <c r="C59" s="3">
-        <v>225.235221</v>
+        <v>141.65</v>
       </c>
       <c r="D59" s="3">
-        <v>-107.529645</v>
+        <v>-117.62</v>
       </c>
       <c r="E59" s="2" t="s">
         <v>259</v>
       </c>
       <c r="F59" s="2">
-        <v>-90</v>
+        <v>0</v>
       </c>
     </row>
     <row r="60" spans="1:6">
       <c r="A60" s="2" t="s">
-        <v>250</v>
+        <v>33</v>
       </c>
       <c r="B60" s="2" t="s">
         <v>149</v>
       </c>
       <c r="C60" s="3">
-        <v>197.567666</v>
+        <v>175.25</v>
       </c>
       <c r="D60" s="3">
-        <v>-102.203459</v>
+        <v>-91.8</v>
       </c>
       <c r="E60" s="2" t="s">
         <v>259</v>
       </c>
       <c r="F60" s="2">
-        <v>-15</v>
+        <v>180</v>
       </c>
     </row>
     <row r="61" spans="1:6">
       <c r="A61" s="2" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="B61" s="2" t="s">
         <v>149</v>
       </c>
       <c r="C61" s="3">
-        <v>141.65</v>
+        <v>123.53740000000001</v>
       </c>
       <c r="D61" s="3">
-        <v>-117.62</v>
+        <v>-130.44540000000001</v>
       </c>
       <c r="E61" s="2" t="s">
         <v>259</v>
       </c>
       <c r="F61" s="2">
-        <v>0</v>
+        <v>105</v>
       </c>
     </row>
     <row r="62" spans="1:6">
       <c r="A62" s="2" t="s">
-        <v>33</v>
+        <v>253</v>
       </c>
       <c r="B62" s="2" t="s">
         <v>149</v>
       </c>
       <c r="C62" s="3">
-        <v>175.25</v>
+        <v>124.7597</v>
       </c>
       <c r="D62" s="3">
-        <v>-91.8</v>
+        <v>-128.89279999999999</v>
       </c>
       <c r="E62" s="2" t="s">
         <v>259</v>
       </c>
       <c r="F62" s="2">
-        <v>180</v>
+        <v>105</v>
       </c>
     </row>
     <row r="63" spans="1:6">
       <c r="A63" s="2" t="s">
-        <v>252</v>
+        <v>43</v>
       </c>
       <c r="B63" s="2" t="s">
         <v>149</v>
       </c>
       <c r="C63" s="3">
-        <v>123.53743299999999</v>
+        <v>123.828</v>
       </c>
       <c r="D63" s="3">
-        <v>-130.44537099999999</v>
+        <v>-125.9455</v>
       </c>
       <c r="E63" s="2" t="s">
         <v>259</v>
@@ -4459,136 +4447,136 @@
     </row>
     <row r="64" spans="1:6">
       <c r="A64" s="2" t="s">
-        <v>253</v>
+        <v>42</v>
       </c>
       <c r="B64" s="2" t="s">
         <v>149</v>
       </c>
       <c r="C64" s="3">
-        <v>124.759731</v>
+        <v>120.7762</v>
       </c>
       <c r="D64" s="3">
-        <v>-128.89282600000001</v>
+        <v>-124.7282</v>
       </c>
       <c r="E64" s="2" t="s">
         <v>259</v>
       </c>
       <c r="F64" s="2">
-        <v>105</v>
+        <v>-165</v>
       </c>
     </row>
     <row r="65" spans="1:6">
       <c r="A65" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B65" s="2" t="s">
         <v>149</v>
       </c>
       <c r="C65" s="3">
-        <v>123.827997</v>
+        <v>140.44399999999999</v>
       </c>
       <c r="D65" s="3">
-        <v>-125.945494</v>
+        <v>-77.650000000000006</v>
       </c>
       <c r="E65" s="2" t="s">
         <v>259</v>
       </c>
       <c r="F65" s="2">
-        <v>105</v>
+        <v>-90</v>
       </c>
     </row>
     <row r="66" spans="1:6">
       <c r="A66" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B66" s="2" t="s">
         <v>149</v>
       </c>
       <c r="C66" s="3">
-        <v>120.776233</v>
+        <v>186.28489999999999</v>
       </c>
       <c r="D66" s="3">
-        <v>-124.728162</v>
+        <v>-127.6306</v>
       </c>
       <c r="E66" s="2" t="s">
         <v>259</v>
       </c>
       <c r="F66" s="2">
-        <v>-165</v>
+        <v>-105</v>
       </c>
     </row>
     <row r="67" spans="1:6">
       <c r="A67" s="2" t="s">
-        <v>41</v>
+        <v>254</v>
       </c>
       <c r="B67" s="2" t="s">
         <v>149</v>
       </c>
       <c r="C67" s="3">
-        <v>140.44399999999999</v>
+        <v>192.0805</v>
       </c>
       <c r="D67" s="3">
-        <v>-77.650000000000006</v>
+        <v>-129.18350000000001</v>
       </c>
       <c r="E67" s="2" t="s">
         <v>259</v>
       </c>
       <c r="F67" s="2">
-        <v>-90</v>
+        <v>-105</v>
       </c>
     </row>
     <row r="68" spans="1:6">
       <c r="A68" s="2" t="s">
-        <v>40</v>
+        <v>56</v>
       </c>
       <c r="B68" s="2" t="s">
         <v>149</v>
       </c>
       <c r="C68" s="3">
-        <v>186.284909</v>
+        <v>178.4</v>
       </c>
       <c r="D68" s="3">
-        <v>-127.63061</v>
+        <v>-91.8</v>
       </c>
       <c r="E68" s="2" t="s">
         <v>259</v>
       </c>
       <c r="F68" s="2">
-        <v>-105</v>
+        <v>0</v>
       </c>
     </row>
     <row r="69" spans="1:6">
       <c r="A69" s="2" t="s">
-        <v>254</v>
+        <v>55</v>
       </c>
       <c r="B69" s="2" t="s">
         <v>149</v>
       </c>
       <c r="C69" s="3">
-        <v>192.08046400000001</v>
+        <v>193.55</v>
       </c>
       <c r="D69" s="3">
-        <v>-129.183525</v>
+        <v>-113.0625</v>
       </c>
       <c r="E69" s="2" t="s">
         <v>259</v>
       </c>
       <c r="F69" s="2">
-        <v>-105</v>
+        <v>90</v>
       </c>
     </row>
     <row r="70" spans="1:6">
       <c r="A70" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B70" s="2" t="s">
         <v>149</v>
       </c>
       <c r="C70" s="3">
-        <v>178.4</v>
+        <v>136.17449999999999</v>
       </c>
       <c r="D70" s="3">
-        <v>-91.8</v>
+        <v>-85.59</v>
       </c>
       <c r="E70" s="2" t="s">
         <v>259</v>
@@ -4599,376 +4587,376 @@
     </row>
     <row r="71" spans="1:6">
       <c r="A71" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B71" s="2" t="s">
         <v>149</v>
       </c>
       <c r="C71" s="3">
-        <v>193.55</v>
+        <v>145.15</v>
       </c>
       <c r="D71" s="3">
-        <v>-113.0625</v>
+        <v>-117.62</v>
       </c>
       <c r="E71" s="2" t="s">
         <v>259</v>
       </c>
       <c r="F71" s="2">
-        <v>90</v>
+        <v>0</v>
       </c>
     </row>
     <row r="72" spans="1:6">
       <c r="A72" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B72" s="2" t="s">
         <v>149</v>
       </c>
       <c r="C72" s="3">
-        <v>136.17449999999999</v>
+        <v>150.69999999999999</v>
       </c>
       <c r="D72" s="3">
-        <v>-85.59</v>
+        <v>-78.900000000000006</v>
       </c>
       <c r="E72" s="2" t="s">
         <v>259</v>
       </c>
       <c r="F72" s="2">
-        <v>0</v>
+        <v>90</v>
       </c>
     </row>
     <row r="73" spans="1:6">
       <c r="A73" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B73" s="2" t="s">
         <v>149</v>
       </c>
       <c r="C73" s="3">
-        <v>145.15</v>
+        <v>136.94999999999999</v>
       </c>
       <c r="D73" s="3">
-        <v>-117.62</v>
+        <v>-124.7</v>
       </c>
       <c r="E73" s="2" t="s">
         <v>259</v>
       </c>
       <c r="F73" s="2">
-        <v>0</v>
+        <v>180</v>
       </c>
     </row>
     <row r="74" spans="1:6">
       <c r="A74" s="2" t="s">
-        <v>52</v>
+        <v>34</v>
       </c>
       <c r="B74" s="2" t="s">
         <v>149</v>
       </c>
       <c r="C74" s="3">
-        <v>150.69999999999999</v>
+        <v>139.30000000000001</v>
       </c>
       <c r="D74" s="3">
-        <v>-78.900000000000006</v>
+        <v>-91.05</v>
       </c>
       <c r="E74" s="2" t="s">
         <v>259</v>
       </c>
       <c r="F74" s="2">
-        <v>90</v>
+        <v>180</v>
       </c>
     </row>
     <row r="75" spans="1:6">
       <c r="A75" s="2" t="s">
-        <v>51</v>
+        <v>92</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C75" s="3">
-        <v>136.94999999999999</v>
+        <v>118.8665</v>
       </c>
       <c r="D75" s="3">
-        <v>-124.7</v>
+        <v>-73.302000000000007</v>
       </c>
       <c r="E75" s="2" t="s">
         <v>259</v>
       </c>
       <c r="F75" s="2">
-        <v>180</v>
+        <v>-152</v>
       </c>
     </row>
     <row r="76" spans="1:6">
       <c r="A76" s="2" t="s">
-        <v>34</v>
+        <v>220</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>149</v>
+        <v>128</v>
       </c>
       <c r="C76" s="3">
-        <v>139.30000000000001</v>
+        <v>105.7931</v>
       </c>
       <c r="D76" s="3">
-        <v>-91.05</v>
+        <v>-91.593100000000007</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>259</v>
+        <v>212</v>
       </c>
       <c r="F76" s="2">
-        <v>180</v>
+        <v>-45</v>
       </c>
     </row>
     <row r="77" spans="1:6">
       <c r="A77" s="2" t="s">
-        <v>92</v>
+        <v>221</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>150</v>
+        <v>128</v>
       </c>
       <c r="C77" s="3">
-        <v>118.866524</v>
+        <v>111.45</v>
       </c>
       <c r="D77" s="3">
-        <v>-73.302024000000003</v>
+        <v>-97.25</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>259</v>
+        <v>212</v>
       </c>
       <c r="F77" s="2">
-        <v>-152</v>
+        <v>-135</v>
       </c>
     </row>
     <row r="78" spans="1:6">
       <c r="A78" s="2" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="B78" s="2" t="s">
         <v>128</v>
       </c>
       <c r="C78" s="3">
-        <v>105.79314599999999</v>
+        <v>100.13630000000001</v>
       </c>
       <c r="D78" s="3">
-        <v>-91.593145000000007</v>
+        <v>-97.25</v>
       </c>
       <c r="E78" s="2" t="s">
         <v>212</v>
       </c>
       <c r="F78" s="2">
-        <v>-45</v>
+        <v>45</v>
       </c>
     </row>
     <row r="79" spans="1:6">
       <c r="A79" s="2" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="B79" s="2" t="s">
         <v>128</v>
       </c>
       <c r="C79" s="3">
-        <v>111.45</v>
+        <v>105.7931</v>
       </c>
       <c r="D79" s="3">
-        <v>-97.25</v>
+        <v>-102.90689999999999</v>
       </c>
       <c r="E79" s="2" t="s">
         <v>212</v>
       </c>
       <c r="F79" s="2">
-        <v>-135</v>
+        <v>135</v>
       </c>
     </row>
     <row r="80" spans="1:6">
       <c r="A80" s="2" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="B80" s="2" t="s">
         <v>128</v>
       </c>
       <c r="C80" s="3">
-        <v>100.136291</v>
+        <v>123.0715</v>
       </c>
       <c r="D80" s="3">
-        <v>-97.25</v>
+        <v>-108.7693</v>
       </c>
       <c r="E80" s="2" t="s">
         <v>212</v>
       </c>
       <c r="F80" s="2">
-        <v>45</v>
+        <v>-170</v>
       </c>
     </row>
     <row r="81" spans="1:6">
       <c r="A81" s="2" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="B81" s="2" t="s">
         <v>128</v>
       </c>
       <c r="C81" s="3">
-        <v>105.79314599999999</v>
+        <v>121.8351</v>
       </c>
       <c r="D81" s="3">
-        <v>-102.906854</v>
+        <v>-101.75749999999999</v>
       </c>
       <c r="E81" s="2" t="s">
         <v>212</v>
       </c>
       <c r="F81" s="2">
-        <v>135</v>
+        <v>-170</v>
       </c>
     </row>
     <row r="82" spans="1:6">
       <c r="A82" s="2" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>128</v>
+        <v>151</v>
       </c>
       <c r="C82" s="3">
-        <v>123.071451</v>
+        <v>183.51900000000001</v>
       </c>
       <c r="D82" s="3">
-        <v>-108.76933200000001</v>
+        <v>-91.519000000000005</v>
       </c>
       <c r="E82" s="2" t="s">
         <v>212</v>
       </c>
       <c r="F82" s="2">
-        <v>-170</v>
+        <v>110</v>
       </c>
     </row>
     <row r="83" spans="1:6">
       <c r="A83" s="2" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>128</v>
+        <v>151</v>
       </c>
       <c r="C83" s="3">
-        <v>121.835076</v>
+        <v>195.119</v>
       </c>
       <c r="D83" s="3">
-        <v>-101.757501</v>
+        <v>-85.968999999999994</v>
       </c>
       <c r="E83" s="2" t="s">
         <v>212</v>
       </c>
       <c r="F83" s="2">
-        <v>-170</v>
+        <v>110</v>
       </c>
     </row>
     <row r="84" spans="1:6">
       <c r="A84" s="2" t="s">
-        <v>226</v>
+        <v>95</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C84" s="3">
-        <v>183.519015</v>
+        <v>123.1681</v>
       </c>
       <c r="D84" s="3">
-        <v>-91.518992999999995</v>
+        <v>-134.76759999999999</v>
       </c>
       <c r="E84" s="2" t="s">
-        <v>212</v>
+        <v>259</v>
       </c>
       <c r="F84" s="2">
-        <v>110</v>
+        <v>-165</v>
       </c>
     </row>
     <row r="85" spans="1:6">
       <c r="A85" s="2" t="s">
-        <v>227</v>
+        <v>96</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>151</v>
+        <v>131</v>
       </c>
       <c r="C85" s="3">
-        <v>195.11901499999999</v>
+        <v>166.34690000000001</v>
       </c>
       <c r="D85" s="3">
-        <v>-85.968992999999998</v>
+        <v>-77.070700000000002</v>
       </c>
       <c r="E85" s="2" t="s">
-        <v>212</v>
+        <v>259</v>
       </c>
       <c r="F85" s="2">
-        <v>110</v>
+        <v>172</v>
       </c>
     </row>
     <row r="86" spans="1:6">
       <c r="A86" s="2" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C86" s="3">
-        <v>123.168148</v>
+        <v>147.88</v>
       </c>
       <c r="D86" s="3">
-        <v>-134.76763800000001</v>
+        <v>-124.5</v>
       </c>
       <c r="E86" s="2" t="s">
         <v>259</v>
       </c>
       <c r="F86" s="2">
-        <v>-165</v>
+        <v>180</v>
       </c>
     </row>
     <row r="87" spans="1:6">
       <c r="A87" s="2" t="s">
-        <v>96</v>
+        <v>36</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>131</v>
+        <v>154</v>
       </c>
       <c r="C87" s="3">
-        <v>166.34687500000001</v>
+        <v>69.033500000000004</v>
       </c>
       <c r="D87" s="3">
-        <v>-77.070689000000002</v>
+        <v>-217.44829999999999</v>
       </c>
       <c r="E87" s="2" t="s">
-        <v>259</v>
+        <v>212</v>
       </c>
       <c r="F87" s="2">
-        <v>172</v>
+        <v>0</v>
       </c>
     </row>
     <row r="88" spans="1:6">
       <c r="A88" s="2" t="s">
-        <v>97</v>
+        <v>37</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="C88" s="3">
-        <v>147.88</v>
+        <v>121.4606</v>
       </c>
       <c r="D88" s="3">
-        <v>-124.5</v>
+        <v>-127.3789</v>
       </c>
       <c r="E88" s="2" t="s">
         <v>259</v>
       </c>
       <c r="F88" s="2">
-        <v>180</v>
+        <v>105</v>
       </c>
     </row>
     <row r="89" spans="1:6">
       <c r="A89" s="2" t="s">
-        <v>36</v>
+        <v>98</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="C89" s="3">
-        <v>69.033475999999993</v>
+        <v>142.30000000000001</v>
       </c>
       <c r="D89" s="3">
-        <v>-217.44825</v>
+        <v>-70.91</v>
       </c>
       <c r="E89" s="2" t="s">
         <v>212</v>
@@ -4979,39 +4967,39 @@
     </row>
     <row r="90" spans="1:6">
       <c r="A90" s="2" t="s">
-        <v>37</v>
+        <v>99</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="C90" s="3">
-        <v>121.46060199999999</v>
+        <v>140.32400000000001</v>
       </c>
       <c r="D90" s="3">
-        <v>-127.37885300000001</v>
+        <v>-122.2735</v>
       </c>
       <c r="E90" s="2" t="s">
         <v>259</v>
       </c>
       <c r="F90" s="2">
-        <v>105</v>
+        <v>180</v>
       </c>
     </row>
     <row r="91" spans="1:6">
       <c r="A91" s="2" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>156</v>
+        <v>35</v>
       </c>
       <c r="C91" s="3">
-        <v>142.30000000000001</v>
+        <v>150.04599999999999</v>
       </c>
       <c r="D91" s="3">
-        <v>-70.91</v>
+        <v>-68.468000000000004</v>
       </c>
       <c r="E91" s="2" t="s">
-        <v>212</v>
+        <v>259</v>
       </c>
       <c r="F91" s="2">
         <v>0</v>
@@ -5019,16 +5007,16 @@
     </row>
     <row r="92" spans="1:6">
       <c r="A92" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C92" s="3">
-        <v>140.32400000000001</v>
+        <v>133.98099999999999</v>
       </c>
       <c r="D92" s="3">
-        <v>-122.2735</v>
+        <v>-89.099000000000004</v>
       </c>
       <c r="E92" s="2" t="s">
         <v>259</v>
@@ -5039,63 +5027,39 @@
     </row>
     <row r="93" spans="1:6">
       <c r="A93" s="2" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>35</v>
+        <v>159</v>
       </c>
       <c r="C93" s="3">
-        <v>150.04599999999999</v>
+        <v>123.0569</v>
       </c>
       <c r="D93" s="3">
-        <v>-68.468000000000004</v>
+        <v>-85.588300000000004</v>
       </c>
       <c r="E93" s="2" t="s">
-        <v>259</v>
+        <v>212</v>
       </c>
       <c r="F93" s="2">
-        <v>0</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="94" spans="1:6">
-      <c r="A94" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="B94" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="C94" s="3">
-        <v>133.98099999999999</v>
-      </c>
-      <c r="D94" s="3">
-        <v>-89.099000000000004</v>
-      </c>
-      <c r="E94" s="2" t="s">
-        <v>259</v>
-      </c>
-      <c r="F94" s="2">
-        <v>180</v>
-      </c>
+      <c r="A94" s="2"/>
+      <c r="B94" s="2"/>
+      <c r="C94" s="3"/>
+      <c r="D94" s="3"/>
+      <c r="E94" s="2"/>
+      <c r="F94" s="2"/>
     </row>
     <row r="95" spans="1:6">
-      <c r="A95" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="B95" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="C95" s="3">
-        <v>123.05685200000001</v>
-      </c>
-      <c r="D95" s="3">
-        <v>-85.588319999999996</v>
-      </c>
-      <c r="E95" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="F95" s="2">
-        <v>-3</v>
-      </c>
+      <c r="A95" s="2"/>
+      <c r="B95" s="2"/>
+      <c r="C95" s="3"/>
+      <c r="D95" s="3"/>
+      <c r="E95" s="2"/>
+      <c r="F95" s="2"/>
     </row>
     <row r="96" spans="1:6">
       <c r="A96" s="2"/>
@@ -5744,22 +5708,6 @@
       <c r="D176" s="3"/>
       <c r="E176" s="2"/>
       <c r="F176" s="2"/>
-    </row>
-    <row r="177" spans="1:6">
-      <c r="A177" s="2"/>
-      <c r="B177" s="2"/>
-      <c r="C177" s="3"/>
-      <c r="D177" s="3"/>
-      <c r="E177" s="2"/>
-      <c r="F177" s="2"/>
-    </row>
-    <row r="178" spans="1:6">
-      <c r="A178" s="2"/>
-      <c r="B178" s="2"/>
-      <c r="C178" s="3"/>
-      <c r="D178" s="3"/>
-      <c r="E178" s="2"/>
-      <c r="F178" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="15" type="noConversion"/>

</xml_diff>